<commit_message>
Add wings and claws logic
</commit_message>
<xml_diff>
--- a/Combiner.Domain/NonDomain/LimbAttributes.xlsx
+++ b/Combiner.Domain/NonDomain/LimbAttributes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8595" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8595" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="10" r:id="rId1"/>
@@ -28,9 +28,10 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'0'!$A$1:$B$23</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'1'!$A$1:$B$91</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2'!$B$1:$B$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'3'!$A$2:$B$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'8'!$A$1:$B$21</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="517">
   <si>
     <t xml:space="preserve">range2_min     </t>
   </si>
@@ -1588,6 +1589,9 @@
   </si>
   <si>
     <t>5Tail</t>
+  </si>
+  <si>
+    <t>MAYBE</t>
   </si>
 </sst>
 </file>
@@ -1834,7 +1838,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1882,11 +1886,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1904,16 +1911,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3620,118 +3617,195 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A20"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>496</v>
+      </c>
+      <c r="B1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" s="23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" s="23" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B12" s="23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B13" s="23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B15" s="23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>288</v>
       </c>
+      <c r="B21" s="23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="23"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="23"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="23"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="23"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="23"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="23"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="23"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="23"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="23"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="23"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="23"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="23"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="23"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="23"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B21">
+    <filterColumn colId="1">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A1:A21">
     <sortCondition ref="A1"/>
   </sortState>
@@ -3743,7 +3817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -4232,7 +4306,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:B91"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
@@ -4799,7 +4873,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A1:B27"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4991,10 +5065,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5026,7 +5101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>150</v>
       </c>
@@ -5047,12 +5122,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>152</v>
       </c>
@@ -5065,52 +5140,52 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>154</v>
       </c>
@@ -5123,7 +5198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>155</v>
       </c>
@@ -5136,27 +5211,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>166</v>
       </c>
@@ -5169,12 +5244,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>153</v>
       </c>
@@ -5183,17 +5258,24 @@
       <c r="A31" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>146</v>
       </c>
-      <c r="B32" t="b">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
-  <sortState ref="A1:A31">
+  <autoFilter ref="A2:B32">
+    <filterColumn colId="1">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
+  <sortState ref="A2:B32">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5868,9 +5950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>